<commit_message>
Update GAA results for 2025-07-05
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G391"/>
+  <dimension ref="A1:G392"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14124,6 +14124,43 @@
         </is>
       </c>
     </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>GAA Hurling All-Ireland Senior Championship</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>05/07/2025</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F392" t="inlineStr">
+        <is>
+          <t>7-26</t>
+        </is>
+      </c>
+      <c r="G392" t="inlineStr">
+        <is>
+          <t>2-21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-07-06
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G392"/>
+  <dimension ref="A1:G394"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14161,6 +14161,80 @@
         </is>
       </c>
     </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>GAA Hurling All-Ireland Senior Championship</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Kilkenny</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>06/07/2025</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F393" t="inlineStr">
+        <is>
+          <t>0-30</t>
+        </is>
+      </c>
+      <c r="G393" t="inlineStr">
+        <is>
+          <t>4-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>2025 Electric Ireland GAA Football All-Ireland Minor Championship</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>06/07/2025</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>Cedral St Conleth's Newbridge</t>
+        </is>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-07-11
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G394"/>
+  <dimension ref="A1:G396"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14235,6 +14235,80 @@
         </is>
       </c>
     </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>GAA Football All-Ireland Junior Championship</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>Warwickshire</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>11/07/2025</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>Abbottstown - GAA Centre of Excellence</t>
+        </is>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>2-12</t>
+        </is>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t>1-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>GAA Football All-Ireland Junior Championship</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Kilkenny</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>11/07/2025</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>Abbottstown - GAA Centre of Excellence</t>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>0-17</t>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-07-12
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G396"/>
+  <dimension ref="A1:G398"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14309,6 +14309,80 @@
         </is>
       </c>
     </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>GAA Football All-Ireland Senior Championship</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>12/07/2025</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>0-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>Tailteann Cup</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>12/07/2025</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>1-24</t>
+        </is>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>2-19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-07-13
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G398"/>
+  <dimension ref="A1:G400"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14383,6 +14383,80 @@
         </is>
       </c>
     </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>GAA Football All-Ireland Senior Championship</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>13/07/2025</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>0-15</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>3-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>GAA Football All-Ireland Junior Championship</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>13/07/2025</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>2-13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-07-21
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1224"/>
+  <dimension ref="A1:G1225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43297,6 +43297,43 @@
         </is>
       </c>
     </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>GAA Hurling All-Ireland Senior Championship</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="D1225" t="inlineStr">
+        <is>
+          <t>20/07/2025</t>
+        </is>
+      </c>
+      <c r="E1225" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1225" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1225" t="inlineStr">
+        <is>
+          <t>3-27</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-07-28
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1815"/>
+  <dimension ref="A1:G1816"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -63984,6 +63984,43 @@
         </is>
       </c>
     </row>
+    <row r="1816">
+      <c r="A1816" t="inlineStr">
+        <is>
+          <t>GAA Football All-Ireland Senior Championship</t>
+        </is>
+      </c>
+      <c r="B1816" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="C1816" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="D1816" t="inlineStr">
+        <is>
+          <t>27/07/2025</t>
+        </is>
+      </c>
+      <c r="E1816" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1816" t="inlineStr">
+        <is>
+          <t>1-26</t>
+        </is>
+      </c>
+      <c r="G1816" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-11-29
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1816"/>
+  <dimension ref="A1:G1817"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64021,6 +64021,43 @@
         </is>
       </c>
     </row>
+    <row r="1817">
+      <c r="A1817" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Junior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1817" t="inlineStr">
+        <is>
+          <t>Thomas McCurtain's GAA Club</t>
+        </is>
+      </c>
+      <c r="C1817" t="inlineStr">
+        <is>
+          <t>Burt</t>
+        </is>
+      </c>
+      <c r="D1817" t="inlineStr">
+        <is>
+          <t>29/11/2025</t>
+        </is>
+      </c>
+      <c r="E1817" t="inlineStr">
+        <is>
+          <t>McGovern Park, Ruislip</t>
+        </is>
+      </c>
+      <c r="F1817" t="inlineStr">
+        <is>
+          <t>0-17</t>
+        </is>
+      </c>
+      <c r="G1817" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-12-06
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1817"/>
+  <dimension ref="A1:G1818"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64058,6 +64058,43 @@
         </is>
       </c>
     </row>
+    <row r="1818">
+      <c r="A1818" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Junior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1818" t="inlineStr">
+        <is>
+          <t>Clogher Eire Óg</t>
+        </is>
+      </c>
+      <c r="C1818" t="inlineStr">
+        <is>
+          <t>Tara GFC</t>
+        </is>
+      </c>
+      <c r="D1818" t="inlineStr">
+        <is>
+          <t>06/12/2025</t>
+        </is>
+      </c>
+      <c r="E1818" t="inlineStr">
+        <is>
+          <t>Mullaghmoyle Park, Stewartstown</t>
+        </is>
+      </c>
+      <c r="F1818" t="inlineStr">
+        <is>
+          <t>2-11</t>
+        </is>
+      </c>
+      <c r="G1818" t="inlineStr">
+        <is>
+          <t>1-13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-12-20
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1818"/>
+  <dimension ref="A1:G1820"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64095,6 +64095,80 @@
         </is>
       </c>
     </row>
+    <row r="1819">
+      <c r="A1819" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Junior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1819" t="inlineStr">
+        <is>
+          <t>Burt</t>
+        </is>
+      </c>
+      <c r="C1819" t="inlineStr">
+        <is>
+          <t>Easkey</t>
+        </is>
+      </c>
+      <c r="D1819" t="inlineStr">
+        <is>
+          <t>20/12/2025</t>
+        </is>
+      </c>
+      <c r="E1819" t="inlineStr">
+        <is>
+          <t>Ballyshannon</t>
+        </is>
+      </c>
+      <c r="F1819" t="inlineStr">
+        <is>
+          <t>1-22</t>
+        </is>
+      </c>
+      <c r="G1819" t="inlineStr">
+        <is>
+          <t>4-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1820">
+      <c r="A1820" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Junior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1820" t="inlineStr">
+        <is>
+          <t>Davidstown Courtnacuddy GAA</t>
+        </is>
+      </c>
+      <c r="C1820" t="inlineStr">
+        <is>
+          <t>Cill Briotáin</t>
+        </is>
+      </c>
+      <c r="D1820" t="inlineStr">
+        <is>
+          <t>20/12/2025</t>
+        </is>
+      </c>
+      <c r="E1820" t="inlineStr">
+        <is>
+          <t>Clonmel</t>
+        </is>
+      </c>
+      <c r="F1820" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+      <c r="G1820" t="inlineStr">
+        <is>
+          <t>2-15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2025-12-21
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1820"/>
+  <dimension ref="A1:G1824"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64169,6 +64169,154 @@
         </is>
       </c>
     </row>
+    <row r="1821">
+      <c r="A1821" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Senior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1821" t="inlineStr">
+        <is>
+          <t>Loughrea</t>
+        </is>
+      </c>
+      <c r="C1821" t="inlineStr">
+        <is>
+          <t>Sleacht Néill</t>
+        </is>
+      </c>
+      <c r="D1821" t="inlineStr">
+        <is>
+          <t>21/12/2025</t>
+        </is>
+      </c>
+      <c r="E1821" t="inlineStr">
+        <is>
+          <t>Parnell Park</t>
+        </is>
+      </c>
+      <c r="F1821" t="inlineStr">
+        <is>
+          <t>2-22</t>
+        </is>
+      </c>
+      <c r="G1821" t="inlineStr">
+        <is>
+          <t>0-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1822">
+      <c r="A1822" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Senior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1822" t="inlineStr">
+        <is>
+          <t>Ballygunner</t>
+        </is>
+      </c>
+      <c r="C1822" t="inlineStr">
+        <is>
+          <t>St Martin's GAA Club</t>
+        </is>
+      </c>
+      <c r="D1822" t="inlineStr">
+        <is>
+          <t>21/12/2025</t>
+        </is>
+      </c>
+      <c r="E1822" t="inlineStr">
+        <is>
+          <t>FBD Semple Stadium, Thurles</t>
+        </is>
+      </c>
+      <c r="F1822" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+      <c r="G1822" t="inlineStr">
+        <is>
+          <t>0-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="1823">
+      <c r="A1823" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Intermediate Club Championship</t>
+        </is>
+      </c>
+      <c r="B1823" t="inlineStr">
+        <is>
+          <t>Tuairín</t>
+        </is>
+      </c>
+      <c r="C1823" t="inlineStr">
+        <is>
+          <t>Éire Óg An Charraig Mhór</t>
+        </is>
+      </c>
+      <c r="D1823" t="inlineStr">
+        <is>
+          <t>21/12/2025</t>
+        </is>
+      </c>
+      <c r="E1823" t="inlineStr">
+        <is>
+          <t>Kingspan Breffni, Cavan</t>
+        </is>
+      </c>
+      <c r="F1823" t="inlineStr">
+        <is>
+          <t>1-28</t>
+        </is>
+      </c>
+      <c r="G1823" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1824">
+      <c r="A1824" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Intermediate Club Championship</t>
+        </is>
+      </c>
+      <c r="B1824" t="inlineStr">
+        <is>
+          <t>Danesfort</t>
+        </is>
+      </c>
+      <c r="C1824" t="inlineStr">
+        <is>
+          <t>Upperchurch-Drombane</t>
+        </is>
+      </c>
+      <c r="D1824" t="inlineStr">
+        <is>
+          <t>21/12/2025</t>
+        </is>
+      </c>
+      <c r="E1824" t="inlineStr">
+        <is>
+          <t>Laois Hire O'Moore Park, Portlaoise</t>
+        </is>
+      </c>
+      <c r="F1824" t="inlineStr">
+        <is>
+          <t>0-14</t>
+        </is>
+      </c>
+      <c r="G1824" t="inlineStr">
+        <is>
+          <t>1-13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-03
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1824"/>
+  <dimension ref="A1:G1829"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64317,6 +64317,191 @@
         </is>
       </c>
     </row>
+    <row r="1825">
+      <c r="A1825" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Senior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1825" t="inlineStr">
+        <is>
+          <t>Ballyboden St Enda's</t>
+        </is>
+      </c>
+      <c r="C1825" t="inlineStr">
+        <is>
+          <t>Dingle</t>
+        </is>
+      </c>
+      <c r="D1825" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="E1825" t="inlineStr">
+        <is>
+          <t>SuperValu Páirc Uí Chaoimh, Cork</t>
+        </is>
+      </c>
+      <c r="F1825" t="inlineStr">
+        <is>
+          <t>1-24</t>
+        </is>
+      </c>
+      <c r="G1825" t="inlineStr">
+        <is>
+          <t>1-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1826">
+      <c r="A1826" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Intermediate Club Championship</t>
+        </is>
+      </c>
+      <c r="B1826" t="inlineStr">
+        <is>
+          <t>Glenullin</t>
+        </is>
+      </c>
+      <c r="C1826" t="inlineStr">
+        <is>
+          <t>Strokestown</t>
+        </is>
+      </c>
+      <c r="D1826" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="E1826" t="inlineStr">
+        <is>
+          <t>Ballyshannon</t>
+        </is>
+      </c>
+      <c r="F1826" t="inlineStr">
+        <is>
+          <t>5-8</t>
+        </is>
+      </c>
+      <c r="G1826" t="inlineStr">
+        <is>
+          <t>2-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1827">
+      <c r="A1827" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Intermediate Club Championship</t>
+        </is>
+      </c>
+      <c r="B1827" t="inlineStr">
+        <is>
+          <t>An Ghaeltacht</t>
+        </is>
+      </c>
+      <c r="C1827" t="inlineStr">
+        <is>
+          <t>Sallins GAA Club</t>
+        </is>
+      </c>
+      <c r="D1827" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="E1827" t="inlineStr">
+        <is>
+          <t>SuperValu Páirc Uí Chaoimh, Cork</t>
+        </is>
+      </c>
+      <c r="F1827" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+      <c r="G1827" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1828">
+      <c r="A1828" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Junior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1828" t="inlineStr">
+        <is>
+          <t>Clogher Eire Óg</t>
+        </is>
+      </c>
+      <c r="C1828" t="inlineStr">
+        <is>
+          <t>Kiltimagh</t>
+        </is>
+      </c>
+      <c r="D1828" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="E1828" t="inlineStr">
+        <is>
+          <t>Heartland Credit Union Páirc Seán MacDiarmada</t>
+        </is>
+      </c>
+      <c r="F1828" t="inlineStr">
+        <is>
+          <t>2-13</t>
+        </is>
+      </c>
+      <c r="G1828" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1829">
+      <c r="A1829" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Junior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1829" t="inlineStr">
+        <is>
+          <t>Ballymacelligott</t>
+        </is>
+      </c>
+      <c r="C1829" t="inlineStr">
+        <is>
+          <t>Grangenolvin</t>
+        </is>
+      </c>
+      <c r="D1829" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="E1829" t="inlineStr">
+        <is>
+          <t>Mick Neville Park Rathkeale</t>
+        </is>
+      </c>
+      <c r="F1829" t="inlineStr">
+        <is>
+          <t>2-13</t>
+        </is>
+      </c>
+      <c r="G1829" t="inlineStr">
+        <is>
+          <t>0-16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-04
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1829"/>
+  <dimension ref="A1:G1830"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64502,6 +64502,43 @@
         </is>
       </c>
     </row>
+    <row r="1830">
+      <c r="A1830" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Senior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1830" t="inlineStr">
+        <is>
+          <t>St Brigids</t>
+        </is>
+      </c>
+      <c r="C1830" t="inlineStr">
+        <is>
+          <t>Scotstown</t>
+        </is>
+      </c>
+      <c r="D1830" t="inlineStr">
+        <is>
+          <t>04/01/2026</t>
+        </is>
+      </c>
+      <c r="E1830" t="inlineStr">
+        <is>
+          <t>Kingspan Breffni, Cavan</t>
+        </is>
+      </c>
+      <c r="F1830" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+      <c r="G1830" t="inlineStr">
+        <is>
+          <t>1-12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-10
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1830"/>
+  <dimension ref="A1:G1832"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64539,6 +64539,80 @@
         </is>
       </c>
     </row>
+    <row r="1831">
+      <c r="A1831" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Intermediate Club Championship</t>
+        </is>
+      </c>
+      <c r="B1831" t="inlineStr">
+        <is>
+          <t>Tuairín</t>
+        </is>
+      </c>
+      <c r="C1831" t="inlineStr">
+        <is>
+          <t>Upperchurch-Drombane</t>
+        </is>
+      </c>
+      <c r="D1831" t="inlineStr">
+        <is>
+          <t>10/01/2026</t>
+        </is>
+      </c>
+      <c r="E1831" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1831" t="inlineStr">
+        <is>
+          <t>2-24</t>
+        </is>
+      </c>
+      <c r="G1831" t="inlineStr">
+        <is>
+          <t>4-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1832">
+      <c r="A1832" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Junior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1832" t="inlineStr">
+        <is>
+          <t>Easkey</t>
+        </is>
+      </c>
+      <c r="C1832" t="inlineStr">
+        <is>
+          <t>Cill Briotáin</t>
+        </is>
+      </c>
+      <c r="D1832" t="inlineStr">
+        <is>
+          <t>10/01/2026</t>
+        </is>
+      </c>
+      <c r="E1832" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1832" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+      <c r="G1832" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-11
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1832"/>
+  <dimension ref="A1:G1833"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64613,6 +64613,43 @@
         </is>
       </c>
     </row>
+    <row r="1833">
+      <c r="A1833" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Junior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1833" t="inlineStr">
+        <is>
+          <t>Ballymacelligott</t>
+        </is>
+      </c>
+      <c r="C1833" t="inlineStr">
+        <is>
+          <t>Clogher Eire Óg</t>
+        </is>
+      </c>
+      <c r="D1833" t="inlineStr">
+        <is>
+          <t>11/01/2026</t>
+        </is>
+      </c>
+      <c r="E1833" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1833" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+      <c r="G1833" t="inlineStr">
+        <is>
+          <t>0-13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-12
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1833"/>
+  <dimension ref="A1:G1834"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64650,6 +64650,43 @@
         </is>
       </c>
     </row>
+    <row r="1834">
+      <c r="A1834" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Intermediate Club Championship</t>
+        </is>
+      </c>
+      <c r="B1834" t="inlineStr">
+        <is>
+          <t>An Ghaeltacht</t>
+        </is>
+      </c>
+      <c r="C1834" t="inlineStr">
+        <is>
+          <t>Glenullin</t>
+        </is>
+      </c>
+      <c r="D1834" t="inlineStr">
+        <is>
+          <t>11/01/2026</t>
+        </is>
+      </c>
+      <c r="E1834" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1834" t="inlineStr">
+        <is>
+          <t>0-12</t>
+        </is>
+      </c>
+      <c r="G1834" t="inlineStr">
+        <is>
+          <t>0-6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-13
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1834"/>
+  <dimension ref="A1:G1836"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64687,6 +64687,80 @@
         </is>
       </c>
     </row>
+    <row r="1835">
+      <c r="A1835" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Intermediate Club Championship</t>
+        </is>
+      </c>
+      <c r="B1835" t="inlineStr">
+        <is>
+          <t>An Ghaeltacht</t>
+        </is>
+      </c>
+      <c r="C1835" t="inlineStr">
+        <is>
+          <t>Sallins</t>
+        </is>
+      </c>
+      <c r="D1835" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="E1835" t="inlineStr">
+        <is>
+          <t>SuperValu Páirc Uí Chaoimh, Cork</t>
+        </is>
+      </c>
+      <c r="F1835" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+      <c r="G1835" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1836">
+      <c r="A1836" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Senior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1836" t="inlineStr">
+        <is>
+          <t>Ballyboden St. Endas</t>
+        </is>
+      </c>
+      <c r="C1836" t="inlineStr">
+        <is>
+          <t>Dingle</t>
+        </is>
+      </c>
+      <c r="D1836" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="E1836" t="inlineStr">
+        <is>
+          <t>SuperValu Páirc Uí Chaoimh, Cork</t>
+        </is>
+      </c>
+      <c r="F1836" t="inlineStr">
+        <is>
+          <t>1-24</t>
+        </is>
+      </c>
+      <c r="G1836" t="inlineStr">
+        <is>
+          <t>1-26</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-19
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1836"/>
+  <dimension ref="A1:G1838"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64761,6 +64761,80 @@
         </is>
       </c>
     </row>
+    <row r="1837">
+      <c r="A1837" t="inlineStr">
+        <is>
+          <t>AIB GAA Football All-Ireland Senior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1837" t="inlineStr">
+        <is>
+          <t>Dingle</t>
+        </is>
+      </c>
+      <c r="C1837" t="inlineStr">
+        <is>
+          <t>St Brigids</t>
+        </is>
+      </c>
+      <c r="D1837" t="inlineStr">
+        <is>
+          <t>18/01/2026</t>
+        </is>
+      </c>
+      <c r="E1837" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1837" t="inlineStr">
+        <is>
+          <t>0-23</t>
+        </is>
+      </c>
+      <c r="G1837" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1838">
+      <c r="A1838" t="inlineStr">
+        <is>
+          <t>AIB GAA Hurling All-Ireland Senior Club Championship</t>
+        </is>
+      </c>
+      <c r="B1838" t="inlineStr">
+        <is>
+          <t>Ballygunner</t>
+        </is>
+      </c>
+      <c r="C1838" t="inlineStr">
+        <is>
+          <t>Loughrea</t>
+        </is>
+      </c>
+      <c r="D1838" t="inlineStr">
+        <is>
+          <t>18/01/2026</t>
+        </is>
+      </c>
+      <c r="E1838" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1838" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+      <c r="G1838" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-24
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1838"/>
+  <dimension ref="A1:G1852"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64823,6 +64823,524 @@
         </is>
       </c>
     </row>
+    <row r="1839">
+      <c r="A1839" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1839" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="C1839" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="D1839" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1839" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1839" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+      <c r="G1839" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1840">
+      <c r="A1840" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1840" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="C1840" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="D1840" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1840" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1840" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+      <c r="G1840" t="inlineStr">
+        <is>
+          <t>1-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1841">
+      <c r="A1841" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1841" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="C1841" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="D1841" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1841" t="inlineStr">
+        <is>
+          <t>O'Neills Healy Park, Omagh</t>
+        </is>
+      </c>
+      <c r="F1841" t="inlineStr">
+        <is>
+          <t>2-16</t>
+        </is>
+      </c>
+      <c r="G1841" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1842">
+      <c r="A1842" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1842" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="C1842" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="D1842" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1842" t="inlineStr">
+        <is>
+          <t>Páirc Esler, Newry</t>
+        </is>
+      </c>
+      <c r="F1842" t="inlineStr">
+        <is>
+          <t>2-19</t>
+        </is>
+      </c>
+      <c r="G1842" t="inlineStr">
+        <is>
+          <t>2-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1843">
+      <c r="A1843" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1843" t="inlineStr">
+        <is>
+          <t>Laois</t>
+        </is>
+      </c>
+      <c r="C1843" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="D1843" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1843" t="inlineStr">
+        <is>
+          <t>Laois Hire O'Moore Park</t>
+        </is>
+      </c>
+      <c r="F1843" t="inlineStr">
+        <is>
+          <t>1-10</t>
+        </is>
+      </c>
+      <c r="G1843" t="inlineStr">
+        <is>
+          <t>0-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1844">
+      <c r="A1844" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1844" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="C1844" t="inlineStr">
+        <is>
+          <t>Galway</t>
+        </is>
+      </c>
+      <c r="D1844" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1844" t="inlineStr">
+        <is>
+          <t>FBD Semple Stadium, Thurles</t>
+        </is>
+      </c>
+      <c r="F1844" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+      <c r="G1844" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1845">
+      <c r="A1845" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1845" t="inlineStr">
+        <is>
+          <t>Carlow</t>
+        </is>
+      </c>
+      <c r="C1845" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="D1845" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1845" t="inlineStr">
+        <is>
+          <t>Netwatch Cullen Park</t>
+        </is>
+      </c>
+      <c r="F1845" t="inlineStr">
+        <is>
+          <t>2-18</t>
+        </is>
+      </c>
+      <c r="G1845" t="inlineStr">
+        <is>
+          <t>1-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1846">
+      <c r="A1846" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1846" t="inlineStr">
+        <is>
+          <t>Wexford</t>
+        </is>
+      </c>
+      <c r="C1846" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="D1846" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1846" t="inlineStr">
+        <is>
+          <t>Chadwicks Wexford Park</t>
+        </is>
+      </c>
+      <c r="F1846" t="inlineStr">
+        <is>
+          <t>1-13</t>
+        </is>
+      </c>
+      <c r="G1846" t="inlineStr">
+        <is>
+          <t>1-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1847">
+      <c r="A1847" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1847" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="C1847" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D1847" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1847" t="inlineStr">
+        <is>
+          <t>Trim</t>
+        </is>
+      </c>
+      <c r="F1847" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+      <c r="G1847" t="inlineStr">
+        <is>
+          <t>1-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="1848">
+      <c r="A1848" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1848" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="C1848" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="D1848" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1848" t="inlineStr">
+        <is>
+          <t>Celtic Park</t>
+        </is>
+      </c>
+      <c r="F1848" t="inlineStr">
+        <is>
+          <t>0-12</t>
+        </is>
+      </c>
+      <c r="G1848" t="inlineStr">
+        <is>
+          <t>5-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1849">
+      <c r="A1849" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1849" t="inlineStr">
+        <is>
+          <t>Armagh</t>
+        </is>
+      </c>
+      <c r="C1849" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="D1849" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1849" t="inlineStr">
+        <is>
+          <t>BOX-IT Athletic Grounds, Armagh</t>
+        </is>
+      </c>
+      <c r="F1849" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1849" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1850">
+      <c r="A1850" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1850" t="inlineStr">
+        <is>
+          <t>Cavan</t>
+        </is>
+      </c>
+      <c r="C1850" t="inlineStr">
+        <is>
+          <t>Warwickshire</t>
+        </is>
+      </c>
+      <c r="D1850" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1850" t="inlineStr">
+        <is>
+          <t>Kingspan Breffni, Cavan</t>
+        </is>
+      </c>
+      <c r="F1850" t="inlineStr">
+        <is>
+          <t>3-13</t>
+        </is>
+      </c>
+      <c r="G1850" t="inlineStr">
+        <is>
+          <t>1-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1851">
+      <c r="A1851" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1851" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="C1851" t="inlineStr">
+        <is>
+          <t>Longford</t>
+        </is>
+      </c>
+      <c r="D1851" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1851" t="inlineStr">
+        <is>
+          <t>Heartland Credit Union Páirc Seán MacDiarmada</t>
+        </is>
+      </c>
+      <c r="F1851" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+      <c r="G1851" t="inlineStr">
+        <is>
+          <t>2-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1852">
+      <c r="A1852" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1852" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="C1852" t="inlineStr">
+        <is>
+          <t>Sligo</t>
+        </is>
+      </c>
+      <c r="D1852" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="E1852" t="inlineStr">
+        <is>
+          <t>Grattan Park, Inniskeen</t>
+        </is>
+      </c>
+      <c r="F1852" t="inlineStr">
+        <is>
+          <t>0-8</t>
+        </is>
+      </c>
+      <c r="G1852" t="inlineStr">
+        <is>
+          <t>2-20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-25
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1852"/>
+  <dimension ref="A1:G1868"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -65341,6 +65341,598 @@
         </is>
       </c>
     </row>
+    <row r="1853">
+      <c r="A1853" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1853" t="inlineStr">
+        <is>
+          <t>Galway</t>
+        </is>
+      </c>
+      <c r="C1853" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+      <c r="D1853" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1853" t="inlineStr">
+        <is>
+          <t>Pearse Stadium</t>
+        </is>
+      </c>
+      <c r="F1853" t="inlineStr">
+        <is>
+          <t>2-18</t>
+        </is>
+      </c>
+      <c r="G1853" t="inlineStr">
+        <is>
+          <t>3-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1854">
+      <c r="A1854" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1854" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="C1854" t="inlineStr">
+        <is>
+          <t>Roscommon</t>
+        </is>
+      </c>
+      <c r="D1854" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1854" t="inlineStr">
+        <is>
+          <t>Fitzgerald Stadium, Killarney</t>
+        </is>
+      </c>
+      <c r="F1854" t="inlineStr">
+        <is>
+          <t>2-18</t>
+        </is>
+      </c>
+      <c r="G1854" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1855">
+      <c r="A1855" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1855" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="C1855" t="inlineStr">
+        <is>
+          <t>Armagh</t>
+        </is>
+      </c>
+      <c r="D1855" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1855" t="inlineStr">
+        <is>
+          <t>St. Tiernach's Park, Clones</t>
+        </is>
+      </c>
+      <c r="F1855" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+      <c r="G1855" t="inlineStr">
+        <is>
+          <t>1-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1856">
+      <c r="A1856" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1856" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="C1856" t="inlineStr">
+        <is>
+          <t>Cavan</t>
+        </is>
+      </c>
+      <c r="D1856" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1856" t="inlineStr">
+        <is>
+          <t>SuperValu Páirc Uí Chaoimh</t>
+        </is>
+      </c>
+      <c r="F1856" t="inlineStr">
+        <is>
+          <t>0-24</t>
+        </is>
+      </c>
+      <c r="G1856" t="inlineStr">
+        <is>
+          <t>2-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1857">
+      <c r="A1857" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1857" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="C1857" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="D1857" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1857" t="inlineStr">
+        <is>
+          <t>Glenisk O'Connor Park</t>
+        </is>
+      </c>
+      <c r="F1857" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+      <c r="G1857" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1858">
+      <c r="A1858" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1858" t="inlineStr">
+        <is>
+          <t>Fermanagh</t>
+        </is>
+      </c>
+      <c r="C1858" t="inlineStr">
+        <is>
+          <t>Wexford</t>
+        </is>
+      </c>
+      <c r="D1858" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1858" t="inlineStr">
+        <is>
+          <t>Brewster Park</t>
+        </is>
+      </c>
+      <c r="F1858" t="inlineStr">
+        <is>
+          <t>0-12</t>
+        </is>
+      </c>
+      <c r="G1858" t="inlineStr">
+        <is>
+          <t>1-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1859">
+      <c r="A1859" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1859" t="inlineStr">
+        <is>
+          <t>Westmeath</t>
+        </is>
+      </c>
+      <c r="C1859" t="inlineStr">
+        <is>
+          <t>Sligo</t>
+        </is>
+      </c>
+      <c r="D1859" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1859" t="inlineStr">
+        <is>
+          <t>TEG Cusack Park</t>
+        </is>
+      </c>
+      <c r="F1859" t="inlineStr">
+        <is>
+          <t>2-14</t>
+        </is>
+      </c>
+      <c r="G1859" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1860">
+      <c r="A1860" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1860" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="C1860" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="D1860" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1860" t="inlineStr">
+        <is>
+          <t>McGovern Park, Ruislip</t>
+        </is>
+      </c>
+      <c r="F1860" t="inlineStr">
+        <is>
+          <t>0-21</t>
+        </is>
+      </c>
+      <c r="G1860" t="inlineStr">
+        <is>
+          <t>0-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1861">
+      <c r="A1861" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1861" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="C1861" t="inlineStr">
+        <is>
+          <t>Carlow</t>
+        </is>
+      </c>
+      <c r="D1861" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1861" t="inlineStr">
+        <is>
+          <t>Roger Casements, Portglenone</t>
+        </is>
+      </c>
+      <c r="F1861" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1861" t="inlineStr">
+        <is>
+          <t>2-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1862">
+      <c r="A1862" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1862" t="inlineStr">
+        <is>
+          <t>Wicklow</t>
+        </is>
+      </c>
+      <c r="C1862" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="D1862" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1862" t="inlineStr">
+        <is>
+          <t>Echelon Park, Aughrim</t>
+        </is>
+      </c>
+      <c r="F1862" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+      <c r="G1862" t="inlineStr">
+        <is>
+          <t>2-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1863">
+      <c r="A1863" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1863" t="inlineStr">
+        <is>
+          <t>Kilkenny</t>
+        </is>
+      </c>
+      <c r="C1863" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="D1863" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1863" t="inlineStr">
+        <is>
+          <t>UPMC Nowlan Park</t>
+        </is>
+      </c>
+      <c r="F1863" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+      <c r="G1863" t="inlineStr">
+        <is>
+          <t>0-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1864">
+      <c r="A1864" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1864" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="C1864" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="D1864" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1864" t="inlineStr">
+        <is>
+          <t>SuperValu Páirc Uí Chaoimh</t>
+        </is>
+      </c>
+      <c r="F1864" t="inlineStr">
+        <is>
+          <t>3-25</t>
+        </is>
+      </c>
+      <c r="G1864" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1865">
+      <c r="A1865" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1865" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="C1865" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="D1865" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1865" t="inlineStr">
+        <is>
+          <t>Zimmer Biomet Páirc Chíosóg, Ennis</t>
+        </is>
+      </c>
+      <c r="F1865" t="inlineStr">
+        <is>
+          <t>3-18</t>
+        </is>
+      </c>
+      <c r="G1865" t="inlineStr">
+        <is>
+          <t>1-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1866">
+      <c r="A1866" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1866" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+      <c r="C1866" t="inlineStr">
+        <is>
+          <t>Laois</t>
+        </is>
+      </c>
+      <c r="D1866" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1866" t="inlineStr">
+        <is>
+          <t>Tooreen (Adrian Freeman Park)</t>
+        </is>
+      </c>
+      <c r="F1866" t="inlineStr">
+        <is>
+          <t>0-12</t>
+        </is>
+      </c>
+      <c r="G1866" t="inlineStr">
+        <is>
+          <t>6-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1867">
+      <c r="A1867" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1867" t="inlineStr">
+        <is>
+          <t>Roscommon</t>
+        </is>
+      </c>
+      <c r="C1867" t="inlineStr">
+        <is>
+          <t>Wicklow</t>
+        </is>
+      </c>
+      <c r="D1867" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1867" t="inlineStr">
+        <is>
+          <t>King &amp; Moffatt Dr. Hyde Park</t>
+        </is>
+      </c>
+      <c r="F1867" t="inlineStr">
+        <is>
+          <t>2-15</t>
+        </is>
+      </c>
+      <c r="G1867" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1868">
+      <c r="A1868" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1868" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="C1868" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="D1868" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="E1868" t="inlineStr">
+        <is>
+          <t>Garvaghey</t>
+        </is>
+      </c>
+      <c r="F1868" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1868" t="inlineStr">
+        <is>
+          <t>3-23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-01-31
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1868"/>
+  <dimension ref="A1:G1881"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -65933,6 +65933,487 @@
         </is>
       </c>
     </row>
+    <row r="1869">
+      <c r="A1869" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1869" t="inlineStr">
+        <is>
+          <t>Armagh</t>
+        </is>
+      </c>
+      <c r="C1869" t="inlineStr">
+        <is>
+          <t>Galway</t>
+        </is>
+      </c>
+      <c r="D1869" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1869" t="inlineStr">
+        <is>
+          <t>BOX-IT Athletic Grounds, Armagh</t>
+        </is>
+      </c>
+      <c r="F1869" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+      <c r="G1869" t="inlineStr">
+        <is>
+          <t>3-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1870">
+      <c r="A1870" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1870" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="C1870" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="D1870" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1870" t="inlineStr">
+        <is>
+          <t>Celtic Park</t>
+        </is>
+      </c>
+      <c r="F1870" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1870" t="inlineStr">
+        <is>
+          <t>1-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1871">
+      <c r="A1871" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1871" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="C1871" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="D1871" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1871" t="inlineStr">
+        <is>
+          <t>Cedral St Conleth's Newbridge</t>
+        </is>
+      </c>
+      <c r="F1871" t="inlineStr">
+        <is>
+          <t>3-17</t>
+        </is>
+      </c>
+      <c r="G1871" t="inlineStr">
+        <is>
+          <t>0-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1872">
+      <c r="A1872" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1872" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="C1872" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="D1872" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1872" t="inlineStr">
+        <is>
+          <t>Mick Neville Park Rathkeale</t>
+        </is>
+      </c>
+      <c r="F1872" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+      <c r="G1872" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1873">
+      <c r="A1873" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1873" t="inlineStr">
+        <is>
+          <t>Wexford</t>
+        </is>
+      </c>
+      <c r="C1873" t="inlineStr">
+        <is>
+          <t>Laois</t>
+        </is>
+      </c>
+      <c r="D1873" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1873" t="inlineStr">
+        <is>
+          <t>Chadwicks Wexford Park</t>
+        </is>
+      </c>
+      <c r="F1873" t="inlineStr">
+        <is>
+          <t>0-23</t>
+        </is>
+      </c>
+      <c r="G1873" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1874">
+      <c r="A1874" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1874" t="inlineStr">
+        <is>
+          <t>Carlow</t>
+        </is>
+      </c>
+      <c r="C1874" t="inlineStr">
+        <is>
+          <t>Wicklow</t>
+        </is>
+      </c>
+      <c r="D1874" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1874" t="inlineStr">
+        <is>
+          <t>Netwatch Cullen Park</t>
+        </is>
+      </c>
+      <c r="F1874" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1874" t="inlineStr">
+        <is>
+          <t>2-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1875">
+      <c r="A1875" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1875" t="inlineStr">
+        <is>
+          <t>Galway</t>
+        </is>
+      </c>
+      <c r="C1875" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="D1875" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1875" t="inlineStr">
+        <is>
+          <t>Pearse Stadium</t>
+        </is>
+      </c>
+      <c r="F1875" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+      <c r="G1875" t="inlineStr">
+        <is>
+          <t>2-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1876">
+      <c r="A1876" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1876" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="C1876" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="D1876" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1876" t="inlineStr">
+        <is>
+          <t>Parnell Park</t>
+        </is>
+      </c>
+      <c r="F1876" t="inlineStr">
+        <is>
+          <t>2-19</t>
+        </is>
+      </c>
+      <c r="G1876" t="inlineStr">
+        <is>
+          <t>0-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1877">
+      <c r="A1877" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1877" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="C1877" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="D1877" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1877" t="inlineStr">
+        <is>
+          <t>Protection &amp; Prosperity Louth GAA Training Centre, Darver</t>
+        </is>
+      </c>
+      <c r="F1877" t="inlineStr">
+        <is>
+          <t>0-16</t>
+        </is>
+      </c>
+      <c r="G1877" t="inlineStr">
+        <is>
+          <t>2-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1878">
+      <c r="A1878" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1878" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="C1878" t="inlineStr">
+        <is>
+          <t>Fermanagh</t>
+        </is>
+      </c>
+      <c r="D1878" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1878" t="inlineStr">
+        <is>
+          <t>Letterkenny</t>
+        </is>
+      </c>
+      <c r="F1878" t="inlineStr">
+        <is>
+          <t>2-35</t>
+        </is>
+      </c>
+      <c r="G1878" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1879">
+      <c r="A1879" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1879" t="inlineStr">
+        <is>
+          <t>Lancashire</t>
+        </is>
+      </c>
+      <c r="C1879" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="D1879" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1879" t="inlineStr">
+        <is>
+          <t>Abbottstown - GAA Centre of Excellence</t>
+        </is>
+      </c>
+      <c r="F1879" t="inlineStr">
+        <is>
+          <t>2-16</t>
+        </is>
+      </c>
+      <c r="G1879" t="inlineStr">
+        <is>
+          <t>1-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1880">
+      <c r="A1880" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1880" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="C1880" t="inlineStr">
+        <is>
+          <t>Sligo</t>
+        </is>
+      </c>
+      <c r="D1880" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1880" t="inlineStr">
+        <is>
+          <t>Heartland Credit Union Páirc Seán MacDiarmada</t>
+        </is>
+      </c>
+      <c r="F1880" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+      <c r="G1880" t="inlineStr">
+        <is>
+          <t>2-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1881">
+      <c r="A1881" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1881" t="inlineStr">
+        <is>
+          <t>Longford</t>
+        </is>
+      </c>
+      <c r="C1881" t="inlineStr">
+        <is>
+          <t>Cavan</t>
+        </is>
+      </c>
+      <c r="D1881" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
+        </is>
+      </c>
+      <c r="E1881" t="inlineStr">
+        <is>
+          <t>Michael Fay Park, Longford Slashers</t>
+        </is>
+      </c>
+      <c r="F1881" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+      <c r="G1881" t="inlineStr">
+        <is>
+          <t>1-12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-02-01
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1881"/>
+  <dimension ref="A1:G1899"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -66414,6 +66414,672 @@
         </is>
       </c>
     </row>
+    <row r="1882">
+      <c r="A1882" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1882" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="C1882" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="D1882" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1882" t="inlineStr">
+        <is>
+          <t>Ballyshannon</t>
+        </is>
+      </c>
+      <c r="F1882" t="inlineStr">
+        <is>
+          <t>1-22</t>
+        </is>
+      </c>
+      <c r="G1882" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1883">
+      <c r="A1883" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1883" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+      <c r="C1883" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="D1883" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1883" t="inlineStr">
+        <is>
+          <t>Hastings Insurance MacHale Park, Castlebar</t>
+        </is>
+      </c>
+      <c r="F1883" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1883" t="inlineStr">
+        <is>
+          <t>2-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1884">
+      <c r="A1884" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1884" t="inlineStr">
+        <is>
+          <t>Roscommon</t>
+        </is>
+      </c>
+      <c r="C1884" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="D1884" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1884" t="inlineStr">
+        <is>
+          <t>King &amp; Moffatt Dr. Hyde Park</t>
+        </is>
+      </c>
+      <c r="F1884" t="inlineStr">
+        <is>
+          <t>3-16</t>
+        </is>
+      </c>
+      <c r="G1884" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1885">
+      <c r="A1885" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1885" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="C1885" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="D1885" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1885" t="inlineStr">
+        <is>
+          <t>Integral GAA Grounds, Drogheda</t>
+        </is>
+      </c>
+      <c r="F1885" t="inlineStr">
+        <is>
+          <t>1-12</t>
+        </is>
+      </c>
+      <c r="G1885" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1886">
+      <c r="A1886" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1886" t="inlineStr">
+        <is>
+          <t>Cavan</t>
+        </is>
+      </c>
+      <c r="C1886" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="D1886" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1886" t="inlineStr">
+        <is>
+          <t>Kingspan Breffni, Cavan</t>
+        </is>
+      </c>
+      <c r="F1886" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1886" t="inlineStr">
+        <is>
+          <t>2-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1887">
+      <c r="A1887" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1887" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="C1887" t="inlineStr">
+        <is>
+          <t>Westmeath</t>
+        </is>
+      </c>
+      <c r="D1887" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1887" t="inlineStr">
+        <is>
+          <t>Zimmer Biomet Páirc Chíosóg, Ennis</t>
+        </is>
+      </c>
+      <c r="F1887" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+      <c r="G1887" t="inlineStr">
+        <is>
+          <t>2-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1888">
+      <c r="A1888" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1888" t="inlineStr">
+        <is>
+          <t>Sligo</t>
+        </is>
+      </c>
+      <c r="C1888" t="inlineStr">
+        <is>
+          <t>Fermanagh</t>
+        </is>
+      </c>
+      <c r="D1888" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1888" t="inlineStr">
+        <is>
+          <t>Markievicz Park, Sligo</t>
+        </is>
+      </c>
+      <c r="F1888" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+      <c r="G1888" t="inlineStr">
+        <is>
+          <t>0-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1889">
+      <c r="A1889" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1889" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="C1889" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="D1889" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1889" t="inlineStr">
+        <is>
+          <t>Heartland Credit Union Páirc Seán MacDiarmada</t>
+        </is>
+      </c>
+      <c r="F1889" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+      <c r="G1889" t="inlineStr">
+        <is>
+          <t>2-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1890">
+      <c r="A1890" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1890" t="inlineStr">
+        <is>
+          <t>Longford</t>
+        </is>
+      </c>
+      <c r="C1890" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D1890" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1890" t="inlineStr">
+        <is>
+          <t>Glennon Brothers Pearse Park</t>
+        </is>
+      </c>
+      <c r="F1890" t="inlineStr">
+        <is>
+          <t>2-8</t>
+        </is>
+      </c>
+      <c r="G1890" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1891">
+      <c r="A1891" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1891" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="C1891" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="D1891" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1891" t="inlineStr">
+        <is>
+          <t>Moneygall</t>
+        </is>
+      </c>
+      <c r="F1891" t="inlineStr">
+        <is>
+          <t>1-13</t>
+        </is>
+      </c>
+      <c r="G1891" t="inlineStr">
+        <is>
+          <t>1-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1892">
+      <c r="A1892" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1892" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="C1892" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="D1892" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1892" t="inlineStr">
+        <is>
+          <t>Glenisk O'Connor Park</t>
+        </is>
+      </c>
+      <c r="F1892" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1892" t="inlineStr">
+        <is>
+          <t>5-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="1893">
+      <c r="A1893" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1893" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="C1893" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="D1893" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1893" t="inlineStr">
+        <is>
+          <t>Azzurri Walsh Park, Waterford</t>
+        </is>
+      </c>
+      <c r="F1893" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+      <c r="G1893" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1894">
+      <c r="A1894" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1894" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="C1894" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="D1894" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1894" t="inlineStr">
+        <is>
+          <t>Rurai Og Cushendall</t>
+        </is>
+      </c>
+      <c r="F1894" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+      <c r="G1894" t="inlineStr">
+        <is>
+          <t>2-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1895">
+      <c r="A1895" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1895" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="C1895" t="inlineStr">
+        <is>
+          <t>Wexford</t>
+        </is>
+      </c>
+      <c r="D1895" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1895" t="inlineStr">
+        <is>
+          <t>Ballycran</t>
+        </is>
+      </c>
+      <c r="F1895" t="inlineStr">
+        <is>
+          <t>0-25</t>
+        </is>
+      </c>
+      <c r="G1895" t="inlineStr">
+        <is>
+          <t>0-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1896">
+      <c r="A1896" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1896" t="inlineStr">
+        <is>
+          <t>Laois</t>
+        </is>
+      </c>
+      <c r="C1896" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="D1896" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1896" t="inlineStr">
+        <is>
+          <t>Laois Hire O'Moore Park</t>
+        </is>
+      </c>
+      <c r="F1896" t="inlineStr">
+        <is>
+          <t>0-25</t>
+        </is>
+      </c>
+      <c r="G1896" t="inlineStr">
+        <is>
+          <t>0-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1897">
+      <c r="A1897" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1897" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="C1897" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+      <c r="D1897" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1897" t="inlineStr">
+        <is>
+          <t>McGovern Park, Ruislip</t>
+        </is>
+      </c>
+      <c r="F1897" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+      <c r="G1897" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1898">
+      <c r="A1898" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1898" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="C1898" t="inlineStr">
+        <is>
+          <t>Westmeath</t>
+        </is>
+      </c>
+      <c r="D1898" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1898" t="inlineStr">
+        <is>
+          <t>Austin Stack Park</t>
+        </is>
+      </c>
+      <c r="F1898" t="inlineStr">
+        <is>
+          <t>2-11</t>
+        </is>
+      </c>
+      <c r="G1898" t="inlineStr">
+        <is>
+          <t>0-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1899">
+      <c r="A1899" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1899" t="inlineStr">
+        <is>
+          <t>Wicklow</t>
+        </is>
+      </c>
+      <c r="C1899" t="inlineStr">
+        <is>
+          <t>Armagh</t>
+        </is>
+      </c>
+      <c r="D1899" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="E1899" t="inlineStr">
+        <is>
+          <t>Echelon Park, Aughrim</t>
+        </is>
+      </c>
+      <c r="F1899" t="inlineStr">
+        <is>
+          <t>2-26</t>
+        </is>
+      </c>
+      <c r="G1899" t="inlineStr">
+        <is>
+          <t>0-10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-02-07
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1899"/>
+  <dimension ref="A1:G1906"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -67080,6 +67080,265 @@
         </is>
       </c>
     </row>
+    <row r="1900">
+      <c r="A1900" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1900" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="C1900" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="D1900" t="inlineStr">
+        <is>
+          <t>07/02/2026</t>
+        </is>
+      </c>
+      <c r="E1900" t="inlineStr">
+        <is>
+          <t>SuperValu Páirc Uí Chaoimh</t>
+        </is>
+      </c>
+      <c r="F1900" t="inlineStr">
+        <is>
+          <t>0-29</t>
+        </is>
+      </c>
+      <c r="G1900" t="inlineStr">
+        <is>
+          <t>0-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1901">
+      <c r="A1901" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1901" t="inlineStr">
+        <is>
+          <t>Wexford</t>
+        </is>
+      </c>
+      <c r="C1901" t="inlineStr">
+        <is>
+          <t>Carlow</t>
+        </is>
+      </c>
+      <c r="D1901" t="inlineStr">
+        <is>
+          <t>07/02/2026</t>
+        </is>
+      </c>
+      <c r="E1901" t="inlineStr">
+        <is>
+          <t>Chadwicks Wexford Park</t>
+        </is>
+      </c>
+      <c r="F1901" t="inlineStr">
+        <is>
+          <t>2-28</t>
+        </is>
+      </c>
+      <c r="G1901" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1902">
+      <c r="A1902" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1902" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="C1902" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D1902" t="inlineStr">
+        <is>
+          <t>07/02/2026</t>
+        </is>
+      </c>
+      <c r="E1902" t="inlineStr">
+        <is>
+          <t>Austin Stack Park</t>
+        </is>
+      </c>
+      <c r="F1902" t="inlineStr">
+        <is>
+          <t>5-21</t>
+        </is>
+      </c>
+      <c r="G1902" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1903">
+      <c r="A1903" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1903" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="C1903" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+      <c r="D1903" t="inlineStr">
+        <is>
+          <t>07/02/2026</t>
+        </is>
+      </c>
+      <c r="E1903" t="inlineStr">
+        <is>
+          <t>Find Insurance Celtic Park, Derry</t>
+        </is>
+      </c>
+      <c r="F1903" t="inlineStr">
+        <is>
+          <t>2-25</t>
+        </is>
+      </c>
+      <c r="G1903" t="inlineStr">
+        <is>
+          <t>0-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1904">
+      <c r="A1904" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1904" t="inlineStr">
+        <is>
+          <t>Armagh</t>
+        </is>
+      </c>
+      <c r="C1904" t="inlineStr">
+        <is>
+          <t>Roscommon</t>
+        </is>
+      </c>
+      <c r="D1904" t="inlineStr">
+        <is>
+          <t>07/02/2026</t>
+        </is>
+      </c>
+      <c r="E1904" t="inlineStr">
+        <is>
+          <t>BOX-IT Athletic Grounds, Armagh</t>
+        </is>
+      </c>
+      <c r="F1904" t="inlineStr">
+        <is>
+          <t>0-12</t>
+        </is>
+      </c>
+      <c r="G1904" t="inlineStr">
+        <is>
+          <t>2-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1905">
+      <c r="A1905" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1905" t="inlineStr">
+        <is>
+          <t>Sligo</t>
+        </is>
+      </c>
+      <c r="C1905" t="inlineStr">
+        <is>
+          <t>Lancashire</t>
+        </is>
+      </c>
+      <c r="D1905" t="inlineStr">
+        <is>
+          <t>07/02/2026</t>
+        </is>
+      </c>
+      <c r="E1905" t="inlineStr">
+        <is>
+          <t>Enniscrone</t>
+        </is>
+      </c>
+      <c r="F1905" t="inlineStr">
+        <is>
+          <t>4-21</t>
+        </is>
+      </c>
+      <c r="G1905" t="inlineStr">
+        <is>
+          <t>1-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1906">
+      <c r="A1906" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1906" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="C1906" t="inlineStr">
+        <is>
+          <t>Longford</t>
+        </is>
+      </c>
+      <c r="D1906" t="inlineStr">
+        <is>
+          <t>07/02/2026</t>
+        </is>
+      </c>
+      <c r="E1906" t="inlineStr">
+        <is>
+          <t>VBC Cloghan, Castleblayney</t>
+        </is>
+      </c>
+      <c r="F1906" t="inlineStr">
+        <is>
+          <t>0-13</t>
+        </is>
+      </c>
+      <c r="G1906" t="inlineStr">
+        <is>
+          <t>1-23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-02-08
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1906"/>
+  <dimension ref="A1:G1915"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -67339,6 +67339,339 @@
         </is>
       </c>
     </row>
+    <row r="1907">
+      <c r="A1907" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1907" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="C1907" t="inlineStr">
+        <is>
+          <t>Longford</t>
+        </is>
+      </c>
+      <c r="D1907" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="E1907" t="inlineStr">
+        <is>
+          <t>Cappoquin Logistics Fraher Field</t>
+        </is>
+      </c>
+      <c r="F1907" t="inlineStr">
+        <is>
+          <t>3-14</t>
+        </is>
+      </c>
+      <c r="G1907" t="inlineStr">
+        <is>
+          <t>2-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1908">
+      <c r="A1908" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1908" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="C1908" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="D1908" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="E1908" t="inlineStr">
+        <is>
+          <t>Azzurri Walsh Park, Waterford</t>
+        </is>
+      </c>
+      <c r="F1908" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+      <c r="G1908" t="inlineStr">
+        <is>
+          <t>0-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1909">
+      <c r="A1909" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1909" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="C1909" t="inlineStr">
+        <is>
+          <t>Kilkenny</t>
+        </is>
+      </c>
+      <c r="D1909" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="E1909" t="inlineStr">
+        <is>
+          <t>TUS Gaelic Grounds</t>
+        </is>
+      </c>
+      <c r="F1909" t="inlineStr">
+        <is>
+          <t>1-26</t>
+        </is>
+      </c>
+      <c r="G1909" t="inlineStr">
+        <is>
+          <t>2-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1910">
+      <c r="A1910" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1910" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="C1910" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="D1910" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="E1910" t="inlineStr">
+        <is>
+          <t>Zimmer Biomet Páirc Chíosóg, Ennis</t>
+        </is>
+      </c>
+      <c r="F1910" t="inlineStr">
+        <is>
+          <t>3-35</t>
+        </is>
+      </c>
+      <c r="G1910" t="inlineStr">
+        <is>
+          <t>0-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1911">
+      <c r="A1911" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1911" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="C1911" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="D1911" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="E1911" t="inlineStr">
+        <is>
+          <t>Cedral St Conleth's Newbridge</t>
+        </is>
+      </c>
+      <c r="F1911" t="inlineStr">
+        <is>
+          <t>3-21</t>
+        </is>
+      </c>
+      <c r="G1911" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1912">
+      <c r="A1912" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1912" t="inlineStr">
+        <is>
+          <t>Westmeath</t>
+        </is>
+      </c>
+      <c r="C1912" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="D1912" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="E1912" t="inlineStr">
+        <is>
+          <t>TEG Cusack Park</t>
+        </is>
+      </c>
+      <c r="F1912" t="inlineStr">
+        <is>
+          <t>0-25</t>
+        </is>
+      </c>
+      <c r="G1912" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1913">
+      <c r="A1913" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1913" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="C1913" t="inlineStr">
+        <is>
+          <t>Wicklow</t>
+        </is>
+      </c>
+      <c r="D1913" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="E1913" t="inlineStr">
+        <is>
+          <t>Garvaghey</t>
+        </is>
+      </c>
+      <c r="F1913" t="inlineStr">
+        <is>
+          <t>0-15</t>
+        </is>
+      </c>
+      <c r="G1913" t="inlineStr">
+        <is>
+          <t>3-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1914">
+      <c r="A1914" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1914" t="inlineStr">
+        <is>
+          <t>Fermanagh</t>
+        </is>
+      </c>
+      <c r="C1914" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="D1914" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="E1914" t="inlineStr">
+        <is>
+          <t>Brewster Park</t>
+        </is>
+      </c>
+      <c r="F1914" t="inlineStr">
+        <is>
+          <t>2-19</t>
+        </is>
+      </c>
+      <c r="G1914" t="inlineStr">
+        <is>
+          <t>3-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1915">
+      <c r="A1915" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1915" t="inlineStr">
+        <is>
+          <t>Warwickshire</t>
+        </is>
+      </c>
+      <c r="C1915" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="D1915" t="inlineStr">
+        <is>
+          <t>08/02/2026</t>
+        </is>
+      </c>
+      <c r="E1915" t="inlineStr">
+        <is>
+          <t>Páirc na hÉireann, Birmingham</t>
+        </is>
+      </c>
+      <c r="F1915" t="inlineStr">
+        <is>
+          <t>2-11</t>
+        </is>
+      </c>
+      <c r="G1915" t="inlineStr">
+        <is>
+          <t>2-29</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-02-14
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1915"/>
+  <dimension ref="A1:G1922"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -67672,6 +67672,265 @@
         </is>
       </c>
     </row>
+    <row r="1916">
+      <c r="A1916" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1916" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="C1916" t="inlineStr">
+        <is>
+          <t>Galway</t>
+        </is>
+      </c>
+      <c r="D1916" t="inlineStr">
+        <is>
+          <t>14/02/2026</t>
+        </is>
+      </c>
+      <c r="E1916" t="inlineStr">
+        <is>
+          <t>Austin Stack Park</t>
+        </is>
+      </c>
+      <c r="F1916" t="inlineStr">
+        <is>
+          <t>2-17</t>
+        </is>
+      </c>
+      <c r="G1916" t="inlineStr">
+        <is>
+          <t>3-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1917">
+      <c r="A1917" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1917" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="C1917" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="D1917" t="inlineStr">
+        <is>
+          <t>14/02/2026</t>
+        </is>
+      </c>
+      <c r="E1917" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1917" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1917" t="inlineStr">
+        <is>
+          <t>0-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1918">
+      <c r="A1918" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1918" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="C1918" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="D1918" t="inlineStr">
+        <is>
+          <t>14/02/2026</t>
+        </is>
+      </c>
+      <c r="E1918" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1918" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+      <c r="G1918" t="inlineStr">
+        <is>
+          <t>0-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1919">
+      <c r="A1919" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1919" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="C1919" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="D1919" t="inlineStr">
+        <is>
+          <t>14/02/2026</t>
+        </is>
+      </c>
+      <c r="E1919" t="inlineStr">
+        <is>
+          <t>Cedral St Conleth's Newbridge</t>
+        </is>
+      </c>
+      <c r="F1919" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1919" t="inlineStr">
+        <is>
+          <t>3-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1920">
+      <c r="A1920" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1920" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="C1920" t="inlineStr">
+        <is>
+          <t>Westmeath</t>
+        </is>
+      </c>
+      <c r="D1920" t="inlineStr">
+        <is>
+          <t>14/02/2026</t>
+        </is>
+      </c>
+      <c r="E1920" t="inlineStr">
+        <is>
+          <t>Páirc Esler, Newry</t>
+        </is>
+      </c>
+      <c r="F1920" t="inlineStr">
+        <is>
+          <t>2-15</t>
+        </is>
+      </c>
+      <c r="G1920" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1921">
+      <c r="A1921" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1921" t="inlineStr">
+        <is>
+          <t>Laois</t>
+        </is>
+      </c>
+      <c r="C1921" t="inlineStr">
+        <is>
+          <t>Sligo</t>
+        </is>
+      </c>
+      <c r="D1921" t="inlineStr">
+        <is>
+          <t>14/02/2026</t>
+        </is>
+      </c>
+      <c r="E1921" t="inlineStr">
+        <is>
+          <t>Laois Hire O'Moore Park</t>
+        </is>
+      </c>
+      <c r="F1921" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+      <c r="G1921" t="inlineStr">
+        <is>
+          <t>1-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1922">
+      <c r="A1922" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1922" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="C1922" t="inlineStr">
+        <is>
+          <t>Wicklow</t>
+        </is>
+      </c>
+      <c r="D1922" t="inlineStr">
+        <is>
+          <t>14/02/2026</t>
+        </is>
+      </c>
+      <c r="E1922" t="inlineStr">
+        <is>
+          <t>Cappoquin Logistics Fraher Field, Dungarvan</t>
+        </is>
+      </c>
+      <c r="F1922" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+      <c r="G1922" t="inlineStr">
+        <is>
+          <t>0-14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-02-15
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1922"/>
+  <dimension ref="A1:G1931"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -67931,6 +67931,339 @@
         </is>
       </c>
     </row>
+    <row r="1923">
+      <c r="A1923" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1923" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="C1923" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+      <c r="D1923" t="inlineStr">
+        <is>
+          <t>15/02/2026</t>
+        </is>
+      </c>
+      <c r="E1923" t="inlineStr">
+        <is>
+          <t>Letterkenny</t>
+        </is>
+      </c>
+      <c r="F1923" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+      <c r="G1923" t="inlineStr">
+        <is>
+          <t>0-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1924">
+      <c r="A1924" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1924" t="inlineStr">
+        <is>
+          <t>Roscommon</t>
+        </is>
+      </c>
+      <c r="C1924" t="inlineStr">
+        <is>
+          <t>Armagh</t>
+        </is>
+      </c>
+      <c r="D1924" t="inlineStr">
+        <is>
+          <t>15/02/2026</t>
+        </is>
+      </c>
+      <c r="E1924" t="inlineStr">
+        <is>
+          <t>King &amp; Moffatt Dr. Hyde Park</t>
+        </is>
+      </c>
+      <c r="F1924" t="inlineStr">
+        <is>
+          <t>3-18</t>
+        </is>
+      </c>
+      <c r="G1924" t="inlineStr">
+        <is>
+          <t>0-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="1925">
+      <c r="A1925" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1925" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="C1925" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="D1925" t="inlineStr">
+        <is>
+          <t>15/02/2026</t>
+        </is>
+      </c>
+      <c r="E1925" t="inlineStr">
+        <is>
+          <t>Glenisk O'Connor Park</t>
+        </is>
+      </c>
+      <c r="F1925" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+      <c r="G1925" t="inlineStr">
+        <is>
+          <t>3-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1926">
+      <c r="A1926" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1926" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="C1926" t="inlineStr">
+        <is>
+          <t>Cavan</t>
+        </is>
+      </c>
+      <c r="D1926" t="inlineStr">
+        <is>
+          <t>15/02/2026</t>
+        </is>
+      </c>
+      <c r="E1926" t="inlineStr">
+        <is>
+          <t>O'Neills Healy Park, Omagh</t>
+        </is>
+      </c>
+      <c r="F1926" t="inlineStr">
+        <is>
+          <t>2-23</t>
+        </is>
+      </c>
+      <c r="G1926" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1927">
+      <c r="A1927" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1927" t="inlineStr">
+        <is>
+          <t>Fermanagh</t>
+        </is>
+      </c>
+      <c r="C1927" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="D1927" t="inlineStr">
+        <is>
+          <t>15/02/2026</t>
+        </is>
+      </c>
+      <c r="E1927" t="inlineStr">
+        <is>
+          <t>Brewster Park</t>
+        </is>
+      </c>
+      <c r="F1927" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+      <c r="G1927" t="inlineStr">
+        <is>
+          <t>2-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1928">
+      <c r="A1928" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1928" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="C1928" t="inlineStr">
+        <is>
+          <t>Wexford</t>
+        </is>
+      </c>
+      <c r="D1928" t="inlineStr">
+        <is>
+          <t>15/02/2026</t>
+        </is>
+      </c>
+      <c r="E1928" t="inlineStr">
+        <is>
+          <t>Mick Neville Park Rathkeale</t>
+        </is>
+      </c>
+      <c r="F1928" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1928" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1929">
+      <c r="A1929" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1929" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="C1929" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="D1929" t="inlineStr">
+        <is>
+          <t>15/02/2026</t>
+        </is>
+      </c>
+      <c r="E1929" t="inlineStr">
+        <is>
+          <t>McGovern Park, Ruislip</t>
+        </is>
+      </c>
+      <c r="F1929" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+      <c r="G1929" t="inlineStr">
+        <is>
+          <t>2-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1930">
+      <c r="A1930" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1930" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="C1930" t="inlineStr">
+        <is>
+          <t>Longford</t>
+        </is>
+      </c>
+      <c r="D1930" t="inlineStr">
+        <is>
+          <t>15/02/2026</t>
+        </is>
+      </c>
+      <c r="E1930" t="inlineStr">
+        <is>
+          <t>Roger Casements, Portglenone</t>
+        </is>
+      </c>
+      <c r="F1930" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+      <c r="G1930" t="inlineStr">
+        <is>
+          <t>1-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1931">
+      <c r="A1931" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1931" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="C1931" t="inlineStr">
+        <is>
+          <t>Carlow</t>
+        </is>
+      </c>
+      <c r="D1931" t="inlineStr">
+        <is>
+          <t>15/02/2026</t>
+        </is>
+      </c>
+      <c r="E1931" t="inlineStr">
+        <is>
+          <t>FBD Semple Stadium, Thurles</t>
+        </is>
+      </c>
+      <c r="F1931" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+      <c r="G1931" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-02-21
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1931"/>
+  <dimension ref="A1:G1945"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -68264,6 +68264,524 @@
         </is>
       </c>
     </row>
+    <row r="1932">
+      <c r="A1932" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1932" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="C1932" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="D1932" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1932" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1932" t="inlineStr">
+        <is>
+          <t>1-10</t>
+        </is>
+      </c>
+      <c r="G1932" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1933">
+      <c r="A1933" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1933" t="inlineStr">
+        <is>
+          <t>Galway</t>
+        </is>
+      </c>
+      <c r="C1933" t="inlineStr">
+        <is>
+          <t>Roscommon</t>
+        </is>
+      </c>
+      <c r="D1933" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1933" t="inlineStr">
+        <is>
+          <t>Pearse Stadium</t>
+        </is>
+      </c>
+      <c r="F1933" t="inlineStr">
+        <is>
+          <t>0-21</t>
+        </is>
+      </c>
+      <c r="G1933" t="inlineStr">
+        <is>
+          <t>2-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1934">
+      <c r="A1934" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1934" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="C1934" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="D1934" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1934" t="inlineStr">
+        <is>
+          <t>Find Insurance Celtic Park, Derry</t>
+        </is>
+      </c>
+      <c r="F1934" t="inlineStr">
+        <is>
+          <t>2-25</t>
+        </is>
+      </c>
+      <c r="G1934" t="inlineStr">
+        <is>
+          <t>0-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1935">
+      <c r="A1935" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1935" t="inlineStr">
+        <is>
+          <t>Carlow</t>
+        </is>
+      </c>
+      <c r="C1935" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="D1935" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1935" t="inlineStr">
+        <is>
+          <t>Netwatch Cullen Park</t>
+        </is>
+      </c>
+      <c r="F1935" t="inlineStr">
+        <is>
+          <t>1-26</t>
+        </is>
+      </c>
+      <c r="G1935" t="inlineStr">
+        <is>
+          <t>0-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1936">
+      <c r="A1936" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1936" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="C1936" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="D1936" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1936" t="inlineStr">
+        <is>
+          <t>FBD Semple Stadium, Thurles</t>
+        </is>
+      </c>
+      <c r="F1936" t="inlineStr">
+        <is>
+          <t>0-21</t>
+        </is>
+      </c>
+      <c r="G1936" t="inlineStr">
+        <is>
+          <t>0-36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1937">
+      <c r="A1937" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1937" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="C1937" t="inlineStr">
+        <is>
+          <t>Wexford</t>
+        </is>
+      </c>
+      <c r="D1937" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1937" t="inlineStr">
+        <is>
+          <t>Páirc an Chrócaigh</t>
+        </is>
+      </c>
+      <c r="F1937" t="inlineStr">
+        <is>
+          <t>4-19</t>
+        </is>
+      </c>
+      <c r="G1937" t="inlineStr">
+        <is>
+          <t>3-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1938">
+      <c r="A1938" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1938" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="C1938" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="D1938" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1938" t="inlineStr">
+        <is>
+          <t>Cedral St Conleth's Newbridge</t>
+        </is>
+      </c>
+      <c r="F1938" t="inlineStr">
+        <is>
+          <t>3-14</t>
+        </is>
+      </c>
+      <c r="G1938" t="inlineStr">
+        <is>
+          <t>0-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1939">
+      <c r="A1939" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1939" t="inlineStr">
+        <is>
+          <t>Laois</t>
+        </is>
+      </c>
+      <c r="C1939" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="D1939" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1939" t="inlineStr">
+        <is>
+          <t>Laois Hire O'Moore Park</t>
+        </is>
+      </c>
+      <c r="F1939" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1939" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1940">
+      <c r="A1940" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1940" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="C1940" t="inlineStr">
+        <is>
+          <t>Armagh</t>
+        </is>
+      </c>
+      <c r="D1940" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1940" t="inlineStr">
+        <is>
+          <t>Letterkenny</t>
+        </is>
+      </c>
+      <c r="F1940" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1940" t="inlineStr">
+        <is>
+          <t>1-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1941">
+      <c r="A1941" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1941" t="inlineStr">
+        <is>
+          <t>Fermanagh</t>
+        </is>
+      </c>
+      <c r="C1941" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="D1941" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1941" t="inlineStr">
+        <is>
+          <t>Brewster Park</t>
+        </is>
+      </c>
+      <c r="F1941" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+      <c r="G1941" t="inlineStr">
+        <is>
+          <t>2-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1942">
+      <c r="A1942" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1942" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="C1942" t="inlineStr">
+        <is>
+          <t>Roscommon</t>
+        </is>
+      </c>
+      <c r="D1942" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1942" t="inlineStr">
+        <is>
+          <t>Protection &amp; Prosperity Louth GAA Training Centre, Darver</t>
+        </is>
+      </c>
+      <c r="F1942" t="inlineStr">
+        <is>
+          <t>0-11</t>
+        </is>
+      </c>
+      <c r="G1942" t="inlineStr">
+        <is>
+          <t>0-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1943">
+      <c r="A1943" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1943" t="inlineStr">
+        <is>
+          <t>Cavan</t>
+        </is>
+      </c>
+      <c r="C1943" t="inlineStr">
+        <is>
+          <t>Lancashire</t>
+        </is>
+      </c>
+      <c r="D1943" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1943" t="inlineStr">
+        <is>
+          <t>Kingspan Breffni, Cavan</t>
+        </is>
+      </c>
+      <c r="F1943" t="inlineStr">
+        <is>
+          <t>2-20</t>
+        </is>
+      </c>
+      <c r="G1943" t="inlineStr">
+        <is>
+          <t>2-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1944">
+      <c r="A1944" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1944" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="C1944" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="D1944" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1944" t="inlineStr">
+        <is>
+          <t>Páirc Grattan, Inniskeen</t>
+        </is>
+      </c>
+      <c r="F1944" t="inlineStr">
+        <is>
+          <t>1-11</t>
+        </is>
+      </c>
+      <c r="G1944" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1945">
+      <c r="A1945" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1945" t="inlineStr">
+        <is>
+          <t>Sligo</t>
+        </is>
+      </c>
+      <c r="C1945" t="inlineStr">
+        <is>
+          <t>Warwickshire</t>
+        </is>
+      </c>
+      <c r="D1945" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1945" t="inlineStr">
+        <is>
+          <t>Tubbercurry</t>
+        </is>
+      </c>
+      <c r="F1945" t="inlineStr">
+        <is>
+          <t>2-34</t>
+        </is>
+      </c>
+      <c r="G1945" t="inlineStr">
+        <is>
+          <t>0-3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-02-22
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1945"/>
+  <dimension ref="A1:G1964"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -68782,6 +68782,709 @@
         </is>
       </c>
     </row>
+    <row r="1946">
+      <c r="A1946" t="inlineStr">
+        <is>
+          <t>Masita GAA Post Primary Schools Croke Cup (Senior A Hurling)</t>
+        </is>
+      </c>
+      <c r="B1946" t="inlineStr">
+        <is>
+          <t>St. Kieran's College</t>
+        </is>
+      </c>
+      <c r="C1946" t="inlineStr">
+        <is>
+          <t>St. Raphael's College Loughrea</t>
+        </is>
+      </c>
+      <c r="D1946" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1946" t="inlineStr">
+        <is>
+          <t>Toomevara, Tipperary</t>
+        </is>
+      </c>
+      <c r="F1946" t="inlineStr">
+        <is>
+          <t>2-19</t>
+        </is>
+      </c>
+      <c r="G1946" t="inlineStr">
+        <is>
+          <t>0-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1947">
+      <c r="A1947" t="inlineStr">
+        <is>
+          <t>Masita GAA Post Primary Schools Croke Cup (Senior A Hurling)</t>
+        </is>
+      </c>
+      <c r="B1947" t="inlineStr">
+        <is>
+          <t>Kilkenny CBS</t>
+        </is>
+      </c>
+      <c r="C1947" t="inlineStr">
+        <is>
+          <t>St. Flannans College Ennis</t>
+        </is>
+      </c>
+      <c r="D1947" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="E1947" t="inlineStr">
+        <is>
+          <t>Bansha</t>
+        </is>
+      </c>
+      <c r="F1947" t="inlineStr">
+        <is>
+          <t>0-13</t>
+        </is>
+      </c>
+      <c r="G1947" t="inlineStr">
+        <is>
+          <t>2-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1948">
+      <c r="A1948" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1948" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="C1948" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+      <c r="D1948" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1948" t="inlineStr">
+        <is>
+          <t>St. Tiernach's Park, Clones</t>
+        </is>
+      </c>
+      <c r="F1948" t="inlineStr">
+        <is>
+          <t>2-11</t>
+        </is>
+      </c>
+      <c r="G1948" t="inlineStr">
+        <is>
+          <t>2-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1949">
+      <c r="A1949" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1949" t="inlineStr">
+        <is>
+          <t>Armagh</t>
+        </is>
+      </c>
+      <c r="C1949" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="D1949" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1949" t="inlineStr">
+        <is>
+          <t>BOX-IT Athletic Grounds, Armagh</t>
+        </is>
+      </c>
+      <c r="F1949" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+      <c r="G1949" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1950">
+      <c r="A1950" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1950" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="C1950" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="D1950" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1950" t="inlineStr">
+        <is>
+          <t>Páirc Uí Rinn</t>
+        </is>
+      </c>
+      <c r="F1950" t="inlineStr">
+        <is>
+          <t>1-23</t>
+        </is>
+      </c>
+      <c r="G1950" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1951">
+      <c r="A1951" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1951" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="C1951" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="D1951" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1951" t="inlineStr">
+        <is>
+          <t>DEFY Pairc Mhuire, Ardee</t>
+        </is>
+      </c>
+      <c r="F1951" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1951" t="inlineStr">
+        <is>
+          <t>0-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1952">
+      <c r="A1952" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1952" t="inlineStr">
+        <is>
+          <t>Cavan</t>
+        </is>
+      </c>
+      <c r="C1952" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="D1952" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1952" t="inlineStr">
+        <is>
+          <t>Kingspan Breffni, Cavan</t>
+        </is>
+      </c>
+      <c r="F1952" t="inlineStr">
+        <is>
+          <t>0-16</t>
+        </is>
+      </c>
+      <c r="G1952" t="inlineStr">
+        <is>
+          <t>0-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1953">
+      <c r="A1953" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1953" t="inlineStr">
+        <is>
+          <t>Sligo</t>
+        </is>
+      </c>
+      <c r="C1953" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="D1953" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1953" t="inlineStr">
+        <is>
+          <t>Markievicz Park, Sligo</t>
+        </is>
+      </c>
+      <c r="F1953" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1953" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1954">
+      <c r="A1954" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1954" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="C1954" t="inlineStr">
+        <is>
+          <t>Laois</t>
+        </is>
+      </c>
+      <c r="D1954" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1954" t="inlineStr">
+        <is>
+          <t>Zimmer Biomet Páirc Chíosóg, Ennis</t>
+        </is>
+      </c>
+      <c r="F1954" t="inlineStr">
+        <is>
+          <t>0-24</t>
+        </is>
+      </c>
+      <c r="G1954" t="inlineStr">
+        <is>
+          <t>2-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1955">
+      <c r="A1955" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1955" t="inlineStr">
+        <is>
+          <t>Westmeath</t>
+        </is>
+      </c>
+      <c r="C1955" t="inlineStr">
+        <is>
+          <t>Fermanagh</t>
+        </is>
+      </c>
+      <c r="D1955" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1955" t="inlineStr">
+        <is>
+          <t>TEG Cusack Park</t>
+        </is>
+      </c>
+      <c r="F1955" t="inlineStr">
+        <is>
+          <t>1-26</t>
+        </is>
+      </c>
+      <c r="G1955" t="inlineStr">
+        <is>
+          <t>2-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1956">
+      <c r="A1956" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1956" t="inlineStr">
+        <is>
+          <t>Wexford</t>
+        </is>
+      </c>
+      <c r="C1956" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="D1956" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1956" t="inlineStr">
+        <is>
+          <t>Chadwicks Wexford Park</t>
+        </is>
+      </c>
+      <c r="F1956" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+      <c r="G1956" t="inlineStr">
+        <is>
+          <t>1-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="1957">
+      <c r="A1957" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1957" t="inlineStr">
+        <is>
+          <t>Wicklow</t>
+        </is>
+      </c>
+      <c r="C1957" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D1957" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1957" t="inlineStr">
+        <is>
+          <t>Echelon Park, Aughrim</t>
+        </is>
+      </c>
+      <c r="F1957" t="inlineStr">
+        <is>
+          <t>2-26</t>
+        </is>
+      </c>
+      <c r="G1957" t="inlineStr">
+        <is>
+          <t>0-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1958">
+      <c r="A1958" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1958" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="C1958" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="D1958" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1958" t="inlineStr">
+        <is>
+          <t>Heartland Credit Union Páirc Seán MacDiarmada</t>
+        </is>
+      </c>
+      <c r="F1958" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1958" t="inlineStr">
+        <is>
+          <t>2-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1959">
+      <c r="A1959" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1959" t="inlineStr">
+        <is>
+          <t>Longford</t>
+        </is>
+      </c>
+      <c r="C1959" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="D1959" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1959" t="inlineStr">
+        <is>
+          <t>Glennon Brothers Pearse Park</t>
+        </is>
+      </c>
+      <c r="F1959" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1959" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1960">
+      <c r="A1960" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1960" t="inlineStr">
+        <is>
+          <t>Kilkenny</t>
+        </is>
+      </c>
+      <c r="C1960" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="D1960" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1960" t="inlineStr">
+        <is>
+          <t>UPMC Nowlan Park</t>
+        </is>
+      </c>
+      <c r="F1960" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+      <c r="G1960" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1961">
+      <c r="A1961" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1961" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="C1961" t="inlineStr">
+        <is>
+          <t>Galway</t>
+        </is>
+      </c>
+      <c r="D1961" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1961" t="inlineStr">
+        <is>
+          <t>Grant Heating St Brendan's Park, Birr</t>
+        </is>
+      </c>
+      <c r="F1961" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+      <c r="G1961" t="inlineStr">
+        <is>
+          <t>2-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1962">
+      <c r="A1962" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1962" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="C1962" t="inlineStr">
+        <is>
+          <t>Carlow</t>
+        </is>
+      </c>
+      <c r="D1962" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1962" t="inlineStr">
+        <is>
+          <t>Corrigan Park</t>
+        </is>
+      </c>
+      <c r="F1962" t="inlineStr">
+        <is>
+          <t>0-25</t>
+        </is>
+      </c>
+      <c r="G1962" t="inlineStr">
+        <is>
+          <t>0-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1963">
+      <c r="A1963" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1963" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="C1963" t="inlineStr">
+        <is>
+          <t>Westmeath</t>
+        </is>
+      </c>
+      <c r="D1963" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1963" t="inlineStr">
+        <is>
+          <t>McGovern Park, Ruislip</t>
+        </is>
+      </c>
+      <c r="F1963" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+      <c r="G1963" t="inlineStr">
+        <is>
+          <t>3-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1964">
+      <c r="A1964" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1964" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="C1964" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="D1964" t="inlineStr">
+        <is>
+          <t>22/02/2026</t>
+        </is>
+      </c>
+      <c r="E1964" t="inlineStr">
+        <is>
+          <t>Trim</t>
+        </is>
+      </c>
+      <c r="F1964" t="inlineStr">
+        <is>
+          <t>1-20</t>
+        </is>
+      </c>
+      <c r="G1964" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-02-28
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1964"/>
+  <dimension ref="A1:G1985"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -69485,6 +69485,779 @@
         </is>
       </c>
     </row>
+    <row r="1965">
+      <c r="A1965" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1965" t="inlineStr">
+        <is>
+          <t>Cavan</t>
+        </is>
+      </c>
+      <c r="C1965" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="D1965" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1965" t="inlineStr">
+        <is>
+          <t>Kingspan Breffni, Cavan</t>
+        </is>
+      </c>
+      <c r="F1965" t="inlineStr">
+        <is>
+          <t>1-12</t>
+        </is>
+      </c>
+      <c r="G1965" t="inlineStr">
+        <is>
+          <t>1-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1966">
+      <c r="A1966" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1966" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="C1966" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="D1966" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1966" t="inlineStr">
+        <is>
+          <t>O Neill Park, Dungannon</t>
+        </is>
+      </c>
+      <c r="F1966" t="inlineStr">
+        <is>
+          <t>0-28</t>
+        </is>
+      </c>
+      <c r="G1966" t="inlineStr">
+        <is>
+          <t>2-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1967">
+      <c r="A1967" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1967" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="C1967" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="D1967" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1967" t="inlineStr">
+        <is>
+          <t>Cedral St Conleth's Newbridge</t>
+        </is>
+      </c>
+      <c r="F1967" t="inlineStr">
+        <is>
+          <t>0-10</t>
+        </is>
+      </c>
+      <c r="G1967" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1968">
+      <c r="A1968" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1968" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="C1968" t="inlineStr">
+        <is>
+          <t>Fermanagh</t>
+        </is>
+      </c>
+      <c r="D1968" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1968" t="inlineStr">
+        <is>
+          <t>Páirc Esler, Newry</t>
+        </is>
+      </c>
+      <c r="F1968" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1968" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1969">
+      <c r="A1969" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1969" t="inlineStr">
+        <is>
+          <t>Laois</t>
+        </is>
+      </c>
+      <c r="C1969" t="inlineStr">
+        <is>
+          <t>Westmeath</t>
+        </is>
+      </c>
+      <c r="D1969" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1969" t="inlineStr">
+        <is>
+          <t>Laois Hire O'Moore Park</t>
+        </is>
+      </c>
+      <c r="F1969" t="inlineStr">
+        <is>
+          <t>3-16</t>
+        </is>
+      </c>
+      <c r="G1969" t="inlineStr">
+        <is>
+          <t>1-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1970">
+      <c r="A1970" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1970" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="C1970" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="D1970" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1970" t="inlineStr">
+        <is>
+          <t>Mick Neville Park Rathkeale</t>
+        </is>
+      </c>
+      <c r="F1970" t="inlineStr">
+        <is>
+          <t>1-12</t>
+        </is>
+      </c>
+      <c r="G1970" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1971">
+      <c r="A1971" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1971" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="C1971" t="inlineStr">
+        <is>
+          <t>Wicklow</t>
+        </is>
+      </c>
+      <c r="D1971" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1971" t="inlineStr">
+        <is>
+          <t>Roger Casements, Portglenone</t>
+        </is>
+      </c>
+      <c r="F1971" t="inlineStr">
+        <is>
+          <t>2-18</t>
+        </is>
+      </c>
+      <c r="G1971" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1972">
+      <c r="A1972" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1972" t="inlineStr">
+        <is>
+          <t>Carlow</t>
+        </is>
+      </c>
+      <c r="C1972" t="inlineStr">
+        <is>
+          <t>Clare</t>
+        </is>
+      </c>
+      <c r="D1972" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1972" t="inlineStr">
+        <is>
+          <t>Netwatch Cullen Park</t>
+        </is>
+      </c>
+      <c r="F1972" t="inlineStr">
+        <is>
+          <t>0-18</t>
+        </is>
+      </c>
+      <c r="G1972" t="inlineStr">
+        <is>
+          <t>1-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="1973">
+      <c r="A1973" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1973" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="C1973" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D1973" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1973" t="inlineStr">
+        <is>
+          <t>Find Insurance Celtic Park, Derry</t>
+        </is>
+      </c>
+      <c r="F1973" t="inlineStr">
+        <is>
+          <t>0-14</t>
+        </is>
+      </c>
+      <c r="G1973" t="inlineStr">
+        <is>
+          <t>3-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1974">
+      <c r="A1974" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1974" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+      <c r="C1974" t="inlineStr">
+        <is>
+          <t>Meath</t>
+        </is>
+      </c>
+      <c r="D1974" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1974" t="inlineStr">
+        <is>
+          <t>Tooreen (Adrian Freeman Park)</t>
+        </is>
+      </c>
+      <c r="F1974" t="inlineStr">
+        <is>
+          <t>1-12</t>
+        </is>
+      </c>
+      <c r="G1974" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1975">
+      <c r="A1975" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1975" t="inlineStr">
+        <is>
+          <t>Roscommon</t>
+        </is>
+      </c>
+      <c r="C1975" t="inlineStr">
+        <is>
+          <t>Tyrone</t>
+        </is>
+      </c>
+      <c r="D1975" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1975" t="inlineStr">
+        <is>
+          <t>King &amp; Moffatt Dr. Hyde Park</t>
+        </is>
+      </c>
+      <c r="F1975" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+      <c r="G1975" t="inlineStr">
+        <is>
+          <t>0-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1976">
+      <c r="A1976" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1976" t="inlineStr">
+        <is>
+          <t>Lancashire</t>
+        </is>
+      </c>
+      <c r="C1976" t="inlineStr">
+        <is>
+          <t>Longford</t>
+        </is>
+      </c>
+      <c r="D1976" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1976" t="inlineStr">
+        <is>
+          <t>Abbottstown - GAA Centre of Excellence</t>
+        </is>
+      </c>
+      <c r="F1976" t="inlineStr">
+        <is>
+          <t>0-12</t>
+        </is>
+      </c>
+      <c r="G1976" t="inlineStr">
+        <is>
+          <t>3-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1977">
+      <c r="A1977" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1977" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="C1977" t="inlineStr">
+        <is>
+          <t>Cavan</t>
+        </is>
+      </c>
+      <c r="D1977" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1977" t="inlineStr">
+        <is>
+          <t>Heartland Credit Union Páirc Seán MacDiarmada</t>
+        </is>
+      </c>
+      <c r="F1977" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+      <c r="G1977" t="inlineStr">
+        <is>
+          <t>0-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1978">
+      <c r="A1978" t="inlineStr">
+        <is>
+          <t>Masita All-Ireland PPS Br Edmund Ignatius Rice Cup (Senior D Football)</t>
+        </is>
+      </c>
+      <c r="B1978" t="inlineStr">
+        <is>
+          <t>Largy College Clones</t>
+        </is>
+      </c>
+      <c r="C1978" t="inlineStr">
+        <is>
+          <t>Mountmellick Community School</t>
+        </is>
+      </c>
+      <c r="D1978" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1978" t="inlineStr"/>
+      <c r="F1978" t="inlineStr">
+        <is>
+          <t>5-15</t>
+        </is>
+      </c>
+      <c r="G1978" t="inlineStr">
+        <is>
+          <t>2-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1979">
+      <c r="A1979" t="inlineStr">
+        <is>
+          <t>Masita All-Ireland PPS Br Edmund Ignatius Rice Cup (Senior D Football)</t>
+        </is>
+      </c>
+      <c r="B1979" t="inlineStr">
+        <is>
+          <t>Rice College Ennis</t>
+        </is>
+      </c>
+      <c r="C1979" t="inlineStr">
+        <is>
+          <t>St. Brendan's College, Belmullet</t>
+        </is>
+      </c>
+      <c r="D1979" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1979" t="inlineStr">
+        <is>
+          <t>Connacht GAA Centre</t>
+        </is>
+      </c>
+      <c r="F1979" t="inlineStr">
+        <is>
+          <t>2-10</t>
+        </is>
+      </c>
+      <c r="G1979" t="inlineStr">
+        <is>
+          <t>2-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1980">
+      <c r="A1980" t="inlineStr">
+        <is>
+          <t>Masita All-Ireland PPS Dr Eamonn O'Sullivan Cup (Senior C Football)</t>
+        </is>
+      </c>
+      <c r="B1980" t="inlineStr">
+        <is>
+          <t>St Ciaran's, Ballygawley</t>
+        </is>
+      </c>
+      <c r="C1980" t="inlineStr">
+        <is>
+          <t>St. Paul's College Raheny</t>
+        </is>
+      </c>
+      <c r="D1980" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1980" t="inlineStr">
+        <is>
+          <t>Crossmaglen</t>
+        </is>
+      </c>
+      <c r="F1980" t="inlineStr">
+        <is>
+          <t>5-20</t>
+        </is>
+      </c>
+      <c r="G1980" t="inlineStr">
+        <is>
+          <t>0-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1981">
+      <c r="A1981" t="inlineStr">
+        <is>
+          <t>Masita All-Ireland PPS Dr Eamonn O'Sullivan Cup (Senior C Football)</t>
+        </is>
+      </c>
+      <c r="B1981" t="inlineStr">
+        <is>
+          <t>Balla Secondary School</t>
+        </is>
+      </c>
+      <c r="C1981" t="inlineStr">
+        <is>
+          <t>Carrigaline Community School</t>
+        </is>
+      </c>
+      <c r="D1981" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1981" t="inlineStr">
+        <is>
+          <t>Clarecastle GAA</t>
+        </is>
+      </c>
+      <c r="F1981" t="inlineStr">
+        <is>
+          <t>3-17</t>
+        </is>
+      </c>
+      <c r="G1981" t="inlineStr">
+        <is>
+          <t>1-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1982">
+      <c r="A1982" t="inlineStr">
+        <is>
+          <t>Masita All-Ireland PPS Hogan Cup (Senior A Football)</t>
+        </is>
+      </c>
+      <c r="B1982" t="inlineStr">
+        <is>
+          <t>St. Gerald's DLS College</t>
+        </is>
+      </c>
+      <c r="C1982" t="inlineStr">
+        <is>
+          <t>Tralee CBS</t>
+        </is>
+      </c>
+      <c r="D1982" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1982" t="inlineStr">
+        <is>
+          <t>TUS Midwest</t>
+        </is>
+      </c>
+      <c r="F1982" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1982" t="inlineStr">
+        <is>
+          <t>4-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1983">
+      <c r="A1983" t="inlineStr">
+        <is>
+          <t>Masita All-Ireland PPS Hogan Cup (Senior A Football)</t>
+        </is>
+      </c>
+      <c r="B1983" t="inlineStr">
+        <is>
+          <t>Colaiste Mhuire Mullingar</t>
+        </is>
+      </c>
+      <c r="C1983" t="inlineStr">
+        <is>
+          <t>Abbey Christian Brothers GS Newry</t>
+        </is>
+      </c>
+      <c r="D1983" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1983" t="inlineStr">
+        <is>
+          <t>Abbottstown - GAA Centre of Excellence</t>
+        </is>
+      </c>
+      <c r="F1983" t="inlineStr">
+        <is>
+          <t>1-23</t>
+        </is>
+      </c>
+      <c r="G1983" t="inlineStr">
+        <is>
+          <t>3-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1984">
+      <c r="A1984" t="inlineStr">
+        <is>
+          <t>Masita All-Ireland PPS Paddy Drummond Cup (Senior B Football)</t>
+        </is>
+      </c>
+      <c r="B1984" t="inlineStr">
+        <is>
+          <t>Aquinas Diocesan GS Belfast</t>
+        </is>
+      </c>
+      <c r="C1984" t="inlineStr">
+        <is>
+          <t>Cnoc Mhuire Granard</t>
+        </is>
+      </c>
+      <c r="D1984" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1984" t="inlineStr">
+        <is>
+          <t>Louis Leonard Memorial Park, Donagh</t>
+        </is>
+      </c>
+      <c r="F1984" t="inlineStr">
+        <is>
+          <t>0-7</t>
+        </is>
+      </c>
+      <c r="G1984" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1985">
+      <c r="A1985" t="inlineStr">
+        <is>
+          <t>Masita All-Ireland PPS Paddy Drummond Cup (Senior B Football)</t>
+        </is>
+      </c>
+      <c r="B1985" t="inlineStr">
+        <is>
+          <t>Mount St. Michael Rosscarbery</t>
+        </is>
+      </c>
+      <c r="C1985" t="inlineStr">
+        <is>
+          <t>St. Nathy's College Ballaghaderreen</t>
+        </is>
+      </c>
+      <c r="D1985" t="inlineStr">
+        <is>
+          <t>28/02/2026</t>
+        </is>
+      </c>
+      <c r="E1985" t="inlineStr">
+        <is>
+          <t>UL Grounds</t>
+        </is>
+      </c>
+      <c r="F1985" t="inlineStr">
+        <is>
+          <t>0-11</t>
+        </is>
+      </c>
+      <c r="G1985" t="inlineStr">
+        <is>
+          <t>3-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GAA results for 2026-03-01
</commit_message>
<xml_diff>
--- a/gaa_results.xlsx
+++ b/gaa_results.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1985"/>
+  <dimension ref="A1:G2003"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -70258,6 +70258,672 @@
         </is>
       </c>
     </row>
+    <row r="1986">
+      <c r="A1986" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1986" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="C1986" t="inlineStr">
+        <is>
+          <t>Galway</t>
+        </is>
+      </c>
+      <c r="D1986" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1986" t="inlineStr">
+        <is>
+          <t>Ballyshannon</t>
+        </is>
+      </c>
+      <c r="F1986" t="inlineStr">
+        <is>
+          <t>1-17</t>
+        </is>
+      </c>
+      <c r="G1986" t="inlineStr">
+        <is>
+          <t>0-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1987">
+      <c r="A1987" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1987" t="inlineStr">
+        <is>
+          <t>Kerry</t>
+        </is>
+      </c>
+      <c r="C1987" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="D1987" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1987" t="inlineStr">
+        <is>
+          <t>Fitzgerald Stadium, Killarney</t>
+        </is>
+      </c>
+      <c r="F1987" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1987" t="inlineStr">
+        <is>
+          <t>0-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1988">
+      <c r="A1988" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1988" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+      <c r="C1988" t="inlineStr">
+        <is>
+          <t>Armagh</t>
+        </is>
+      </c>
+      <c r="D1988" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1988" t="inlineStr">
+        <is>
+          <t>Hastings Insurance MacHale Park, Castlebar</t>
+        </is>
+      </c>
+      <c r="F1988" t="inlineStr">
+        <is>
+          <t>2-17</t>
+        </is>
+      </c>
+      <c r="G1988" t="inlineStr">
+        <is>
+          <t>0-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1989">
+      <c r="A1989" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 1</t>
+        </is>
+      </c>
+      <c r="B1989" t="inlineStr">
+        <is>
+          <t>Roscommon</t>
+        </is>
+      </c>
+      <c r="C1989" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="D1989" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1989" t="inlineStr">
+        <is>
+          <t>King &amp; Moffatt Dr. Hyde Park</t>
+        </is>
+      </c>
+      <c r="F1989" t="inlineStr">
+        <is>
+          <t>2-7</t>
+        </is>
+      </c>
+      <c r="G1989" t="inlineStr">
+        <is>
+          <t>1-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1990">
+      <c r="A1990" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B1990" t="inlineStr">
+        <is>
+          <t>Derry</t>
+        </is>
+      </c>
+      <c r="C1990" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="D1990" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1990" t="inlineStr">
+        <is>
+          <t>Find Insurance Celtic Park, Derry</t>
+        </is>
+      </c>
+      <c r="F1990" t="inlineStr">
+        <is>
+          <t>1-31</t>
+        </is>
+      </c>
+      <c r="G1990" t="inlineStr">
+        <is>
+          <t>0-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1991">
+      <c r="A1991" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B1991" t="inlineStr">
+        <is>
+          <t>Wexford</t>
+        </is>
+      </c>
+      <c r="C1991" t="inlineStr">
+        <is>
+          <t>Sligo</t>
+        </is>
+      </c>
+      <c r="D1991" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1991" t="inlineStr">
+        <is>
+          <t>Chadwicks Wexford Park</t>
+        </is>
+      </c>
+      <c r="F1991" t="inlineStr">
+        <is>
+          <t>0-16</t>
+        </is>
+      </c>
+      <c r="G1991" t="inlineStr">
+        <is>
+          <t>1-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1992">
+      <c r="A1992" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1992" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="C1992" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="D1992" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1992" t="inlineStr">
+        <is>
+          <t>McGovern Park, Ruislip</t>
+        </is>
+      </c>
+      <c r="F1992" t="inlineStr">
+        <is>
+          <t>3-16</t>
+        </is>
+      </c>
+      <c r="G1992" t="inlineStr">
+        <is>
+          <t>2-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1993">
+      <c r="A1993" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1993" t="inlineStr">
+        <is>
+          <t>Longford</t>
+        </is>
+      </c>
+      <c r="C1993" t="inlineStr">
+        <is>
+          <t>Carlow</t>
+        </is>
+      </c>
+      <c r="D1993" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1993" t="inlineStr">
+        <is>
+          <t>Glennon Brothers Pearse Park</t>
+        </is>
+      </c>
+      <c r="F1993" t="inlineStr">
+        <is>
+          <t>1-19</t>
+        </is>
+      </c>
+      <c r="G1993" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1994">
+      <c r="A1994" t="inlineStr">
+        <is>
+          <t>Allianz Football League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B1994" t="inlineStr">
+        <is>
+          <t>Tipperary</t>
+        </is>
+      </c>
+      <c r="C1994" t="inlineStr">
+        <is>
+          <t>Leitrim</t>
+        </is>
+      </c>
+      <c r="D1994" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1994" t="inlineStr">
+        <is>
+          <t>Clonmel</t>
+        </is>
+      </c>
+      <c r="F1994" t="inlineStr">
+        <is>
+          <t>1-18</t>
+        </is>
+      </c>
+      <c r="G1994" t="inlineStr">
+        <is>
+          <t>0-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1995">
+      <c r="A1995" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1995" t="inlineStr">
+        <is>
+          <t>Galway</t>
+        </is>
+      </c>
+      <c r="C1995" t="inlineStr">
+        <is>
+          <t>Waterford</t>
+        </is>
+      </c>
+      <c r="D1995" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1995" t="inlineStr">
+        <is>
+          <t>Pearse Stadium</t>
+        </is>
+      </c>
+      <c r="F1995" t="inlineStr">
+        <is>
+          <t>2-18</t>
+        </is>
+      </c>
+      <c r="G1995" t="inlineStr">
+        <is>
+          <t>0-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1996">
+      <c r="A1996" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1996" t="inlineStr">
+        <is>
+          <t>Offaly</t>
+        </is>
+      </c>
+      <c r="C1996" t="inlineStr">
+        <is>
+          <t>Limerick</t>
+        </is>
+      </c>
+      <c r="D1996" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1996" t="inlineStr">
+        <is>
+          <t>Glenisk O'Connor Park</t>
+        </is>
+      </c>
+      <c r="F1996" t="inlineStr">
+        <is>
+          <t>0-17</t>
+        </is>
+      </c>
+      <c r="G1996" t="inlineStr">
+        <is>
+          <t>2-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1997">
+      <c r="A1997" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1A</t>
+        </is>
+      </c>
+      <c r="B1997" t="inlineStr">
+        <is>
+          <t>Kilkenny</t>
+        </is>
+      </c>
+      <c r="C1997" t="inlineStr">
+        <is>
+          <t>Cork</t>
+        </is>
+      </c>
+      <c r="D1997" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1997" t="inlineStr">
+        <is>
+          <t>UPMC Nowlan Park</t>
+        </is>
+      </c>
+      <c r="F1997" t="inlineStr">
+        <is>
+          <t>1-15</t>
+        </is>
+      </c>
+      <c r="G1997" t="inlineStr">
+        <is>
+          <t>3-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1998">
+      <c r="A1998" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1998" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="C1998" t="inlineStr">
+        <is>
+          <t>Kildare</t>
+        </is>
+      </c>
+      <c r="D1998" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1998" t="inlineStr">
+        <is>
+          <t>Fontenoy Park, Liatroim Co. Down</t>
+        </is>
+      </c>
+      <c r="F1998" t="inlineStr">
+        <is>
+          <t>1-23</t>
+        </is>
+      </c>
+      <c r="G1998" t="inlineStr">
+        <is>
+          <t>3-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="1999">
+      <c r="A1999" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 1B</t>
+        </is>
+      </c>
+      <c r="B1999" t="inlineStr">
+        <is>
+          <t>Antrim</t>
+        </is>
+      </c>
+      <c r="C1999" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+      <c r="D1999" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E1999" t="inlineStr">
+        <is>
+          <t>Corrigan Park</t>
+        </is>
+      </c>
+      <c r="F1999" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+      <c r="G1999" t="inlineStr">
+        <is>
+          <t>1-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="2000">
+      <c r="A2000" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 2</t>
+        </is>
+      </c>
+      <c r="B2000" t="inlineStr">
+        <is>
+          <t>Westmeath</t>
+        </is>
+      </c>
+      <c r="C2000" t="inlineStr">
+        <is>
+          <t>Laois</t>
+        </is>
+      </c>
+      <c r="D2000" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E2000" t="inlineStr">
+        <is>
+          <t>TEG Cusack Park</t>
+        </is>
+      </c>
+      <c r="F2000" t="inlineStr">
+        <is>
+          <t>0-17</t>
+        </is>
+      </c>
+      <c r="G2000" t="inlineStr">
+        <is>
+          <t>1-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2001">
+      <c r="A2001" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B2001" t="inlineStr">
+        <is>
+          <t>Louth</t>
+        </is>
+      </c>
+      <c r="C2001" t="inlineStr">
+        <is>
+          <t>Donegal</t>
+        </is>
+      </c>
+      <c r="D2001" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E2001" t="inlineStr">
+        <is>
+          <t>Protection &amp; Prosperity Louth GAA Training Centre, Darver</t>
+        </is>
+      </c>
+      <c r="F2001" t="inlineStr">
+        <is>
+          <t>1-9</t>
+        </is>
+      </c>
+      <c r="G2001" t="inlineStr">
+        <is>
+          <t>3-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="2002">
+      <c r="A2002" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 3</t>
+        </is>
+      </c>
+      <c r="B2002" t="inlineStr">
+        <is>
+          <t>Wicklow</t>
+        </is>
+      </c>
+      <c r="C2002" t="inlineStr">
+        <is>
+          <t>Fermanagh</t>
+        </is>
+      </c>
+      <c r="D2002" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E2002" t="inlineStr">
+        <is>
+          <t>Echelon Park, Aughrim</t>
+        </is>
+      </c>
+      <c r="F2002" t="inlineStr">
+        <is>
+          <t>5-14</t>
+        </is>
+      </c>
+      <c r="G2002" t="inlineStr">
+        <is>
+          <t>0-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="2003">
+      <c r="A2003" t="inlineStr">
+        <is>
+          <t>Allianz Hurling League Roinn 4</t>
+        </is>
+      </c>
+      <c r="B2003" t="inlineStr">
+        <is>
+          <t>Warwickshire</t>
+        </is>
+      </c>
+      <c r="C2003" t="inlineStr">
+        <is>
+          <t>Monaghan</t>
+        </is>
+      </c>
+      <c r="D2003" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="E2003" t="inlineStr">
+        <is>
+          <t>Páirc na hÉireann, Birmingham</t>
+        </is>
+      </c>
+      <c r="F2003" t="inlineStr">
+        <is>
+          <t>3-11</t>
+        </is>
+      </c>
+      <c r="G2003" t="inlineStr">
+        <is>
+          <t>0-13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>